<commit_message>
new design + port table
</commit_message>
<xml_diff>
--- a/IPAM Network.xlsx
+++ b/IPAM Network.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Providing-Networks-and-Services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C79FB6F-FE96-4805-9135-0C01E40F74AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5C5B0E-A272-4398-A768-89DEFDE002C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="1" xr2:uid="{11A0E738-140A-4964-9A44-6C448A1CB627}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="2" xr2:uid="{11A0E738-140A-4964-9A44-6C448A1CB627}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Ports" sheetId="2" r:id="rId2"/>
+    <sheet name="old" sheetId="1" r:id="rId1"/>
+    <sheet name="Port table" sheetId="2" r:id="rId2"/>
+    <sheet name="IPAM" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="92">
   <si>
     <t>Clients</t>
   </si>
@@ -375,7 +376,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,8 +419,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -556,11 +563,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -599,27 +635,81 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1754,8 +1844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8964BE-EB3F-4EE5-94B0-FC75935E9F6E}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1769,13 +1859,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.4">
@@ -1895,13 +1985,13 @@
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.4">
@@ -2126,14 +2216,14 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
     </row>
     <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.4">
       <c r="A25" s="8" t="s">
@@ -2228,14 +2318,14 @@
       <c r="F32" s="27"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="38" t="s">
+      <c r="A33" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
     </row>
     <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.4">
       <c r="A34" s="35" t="s">
@@ -2318,9 +2408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C5B68B-7A50-48B3-8148-501BEE13B4B8}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+    <sheetView zoomScale="101" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2331,149 +2421,175 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="41"/>
-      <c r="B4" t="s">
+      <c r="A4" s="48"/>
+      <c r="B4" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="42" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
+      <c r="A5" s="50"/>
+      <c r="B5" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="42" t="s">
         <v>74</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="50"/>
+      <c r="B6" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="49"/>
+      <c r="C7" s="42"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="50"/>
+      <c r="B8" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>86</v>
+      </c>
+    </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
+      <c r="A9" s="50"/>
+      <c r="B9" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="50"/>
+      <c r="B10" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="42" t="s">
-        <v>20</v>
-      </c>
+      <c r="A11" s="50"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="42"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
+      <c r="A12" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="49"/>
+      <c r="C12" s="42"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="50"/>
+      <c r="B13" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="C12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" t="s">
-        <v>88</v>
+      <c r="C13" s="42" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+      <c r="A14" s="50"/>
+      <c r="B14" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="C14" t="s">
-        <v>85</v>
-      </c>
+      <c r="C14" s="42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="50"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="42"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="44" t="s">
-        <v>22</v>
-      </c>
+      <c r="A16" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="49"/>
+      <c r="C16" s="42"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
+      <c r="A17" s="50"/>
+      <c r="B17" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="C17" t="s">
-        <v>89</v>
+      <c r="C17" s="42" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
+      <c r="A18" s="53"/>
+      <c r="B18" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="C18" t="s">
-        <v>45</v>
+      <c r="C18" s="44" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" t="s">
-        <v>51</v>
-      </c>
-    </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="66"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="39" t="s">
         <v>31</v>
       </c>
+      <c r="C25" s="12"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>81</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="42" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2481,7 +2597,7 @@
       <c r="B27" t="s">
         <v>82</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="42" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2489,7 +2605,7 @@
       <c r="B28" t="s">
         <v>83</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="42" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2497,20 +2613,24 @@
       <c r="B29" t="s">
         <v>84</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="42" t="s">
         <v>18</v>
       </c>
     </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C30" s="42"/>
+    </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="39" t="s">
         <v>39</v>
       </c>
+      <c r="C31" s="42"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>81</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="42" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2518,7 +2638,7 @@
       <c r="B33" t="s">
         <v>82</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="42" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2526,7 +2646,7 @@
       <c r="B34" t="s">
         <v>83</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="42" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2534,20 +2654,24 @@
       <c r="B35" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="43" t="s">
+      <c r="C35" s="42" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C36" s="42"/>
+    </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="42" t="s">
+      <c r="A37" s="39" t="s">
         <v>45</v>
       </c>
+      <c r="C37" s="42"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>82</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="42" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2555,7 +2679,7 @@
       <c r="B39" t="s">
         <v>81</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="42" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2563,7 +2687,7 @@
       <c r="B40" t="s">
         <v>83</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="42" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2571,20 +2695,24 @@
       <c r="B41" t="s">
         <v>85</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="42" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C42" s="42"/>
+    </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="42" t="s">
+      <c r="A43" s="39" t="s">
         <v>51</v>
       </c>
+      <c r="C43" s="42"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>82</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="42" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2592,7 +2720,7 @@
       <c r="B45" t="s">
         <v>81</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="42" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2600,15 +2728,16 @@
       <c r="B46" t="s">
         <v>83</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="42" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B47" t="s">
+      <c r="A47" s="43"/>
+      <c r="B47" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="44" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2620,4 +2749,521 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7559BD21-F230-4BA5-919B-45F3A616B79F}">
+  <dimension ref="A1:F39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="18.36328125" customWidth="1"/>
+    <col min="4" max="4" width="19.36328125" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" customWidth="1"/>
+    <col min="6" max="6" width="7.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="58"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="64" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="42">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="44">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="58"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="61" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="50"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="42">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="53"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="44">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="50"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="42"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="50"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="53"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="44">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="50"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="42"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="50"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="42">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="53"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="44">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="50"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="42"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="50"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="42">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="53"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="44">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="69"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="64" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="71"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="73"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="54"/>
+      <c r="C30" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="49"/>
+      <c r="C31" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="49"/>
+      <c r="C32" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="58"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="64" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="54"/>
+      <c r="C38" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="54"/>
+      <c r="F38" s="12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="43"/>
+      <c r="C39" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="43"/>
+      <c r="F39" s="44">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A9:F9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
IPAM rectification of an error
</commit_message>
<xml_diff>
--- a/IPAM Network.xlsx
+++ b/IPAM Network.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Providing-Networks-and-Services\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaiwi\Desktop\Projekte\Netzwerke\Providing-Networks-and-Services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5C5B0E-A272-4398-A768-89DEFDE002C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD63B0AF-6253-4BDF-A98B-30A13047C6F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="2" xr2:uid="{11A0E738-140A-4964-9A44-6C448A1CB627}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{11A0E738-140A-4964-9A44-6C448A1CB627}"/>
   </bookViews>
   <sheets>
     <sheet name="old" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="95">
   <si>
     <t>Clients</t>
   </si>
@@ -312,6 +312,15 @@
   </si>
   <si>
     <t>Switch</t>
+  </si>
+  <si>
+    <t>fda2:b195:3:30::4</t>
+  </si>
+  <si>
+    <t>2001:db8:02:30::100</t>
+  </si>
+  <si>
+    <t>2001:db8:02:40::100</t>
   </si>
 </sst>
 </file>
@@ -596,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -641,12 +650,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -660,7 +663,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -671,6 +673,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -680,34 +704,11 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1848,27 +1849,27 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.54296875" customWidth="1"/>
-    <col min="2" max="2" width="31.54296875" customWidth="1"/>
-    <col min="3" max="3" width="38.7265625" customWidth="1"/>
-    <col min="4" max="4" width="22.54296875" customWidth="1"/>
-    <col min="5" max="5" width="22.7265625" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -1888,7 +1889,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>7</v>
       </c>
@@ -1906,7 +1907,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -1924,7 +1925,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
@@ -1942,7 +1943,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
@@ -1960,7 +1961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1968,7 +1969,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1976,7 +1977,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="16"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -1984,17 +1985,17 @@
       <c r="E9" s="17"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="41" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
         <v>3</v>
       </c>
@@ -2015,7 +2016,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>31</v>
       </c>
@@ -2033,7 +2034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
@@ -2049,7 +2050,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="31"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32" t="s">
@@ -2065,7 +2066,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>39</v>
       </c>
@@ -2083,7 +2084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32" t="s">
@@ -2099,7 +2100,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
@@ -2115,7 +2116,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>45</v>
       </c>
@@ -2133,7 +2134,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
@@ -2149,7 +2150,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="31"/>
       <c r="B20" s="32"/>
       <c r="C20" s="32" t="s">
@@ -2165,7 +2166,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>51</v>
       </c>
@@ -2183,7 +2184,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="31"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32" t="s">
@@ -2199,7 +2200,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21" t="s">
@@ -2215,17 +2216,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="41" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-    </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>3</v>
       </c>
@@ -2245,7 +2246,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>18</v>
       </c>
@@ -2257,7 +2258,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="15"/>
     </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>20</v>
       </c>
@@ -2269,7 +2270,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="15"/>
     </row>
-    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>22</v>
       </c>
@@ -2281,7 +2282,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="15"/>
     </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>23</v>
       </c>
@@ -2293,7 +2294,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="15"/>
     </row>
-    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2301,7 +2302,7 @@
       <c r="E30" s="5"/>
       <c r="F30" s="15"/>
     </row>
-    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2309,7 +2310,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="15"/>
     </row>
-    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
@@ -2317,17 +2318,17 @@
       <c r="E32" s="26"/>
       <c r="F32" s="27"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="40" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-    </row>
-    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="35" t="s">
         <v>3</v>
       </c>
@@ -2347,7 +2348,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>27</v>
       </c>
@@ -2363,7 +2364,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="37" t="s">
         <v>29</v>
       </c>
@@ -2379,7 +2380,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -2409,335 +2410,330 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.36328125" customWidth="1"/>
-    <col min="2" max="2" width="17.08984375" customWidth="1"/>
-    <col min="3" max="3" width="22.90625" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="56" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="38"/>
       <c r="E1" s="38"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="66" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="45" t="s">
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="48"/>
-      <c r="B4" s="49" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="45"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="46"/>
+      <c r="B4" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="40" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="50"/>
-      <c r="B5" s="49" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="47"/>
+      <c r="B5" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="40" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="50"/>
-      <c r="B6" s="49" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="47"/>
+      <c r="B6" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="40" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="51" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="42"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="50"/>
-      <c r="B8" s="49" t="s">
+      <c r="C7" s="40"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="47"/>
+      <c r="B8" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="40" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="50"/>
-      <c r="B9" s="49" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="47"/>
+      <c r="B9" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="40" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="50"/>
-      <c r="B10" s="49" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="47"/>
+      <c r="B10" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="40" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="50"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="42"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="52" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="47"/>
+      <c r="C11" s="40"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="49"/>
-      <c r="C12" s="42"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="50"/>
-      <c r="B13" s="49" t="s">
+      <c r="C12" s="40"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
+      <c r="B13" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="40" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="50"/>
-      <c r="B14" s="49" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="47"/>
+      <c r="B14" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="50"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="42"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="51" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="47"/>
+      <c r="C15" s="40"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="42"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="50"/>
-      <c r="B17" s="49" t="s">
+      <c r="C16" s="40"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="47"/>
+      <c r="B17" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="40" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="53"/>
-      <c r="B18" s="43" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="50"/>
+      <c r="B18" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="42" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E19" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="66" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="66"/>
-      <c r="C24" s="66"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="39" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="12"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="40" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="40" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C30" s="42"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="40"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="42"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C31" s="40"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="40" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="40" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="42" t="s">
+      <c r="C34" s="40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="42" t="s">
+      <c r="C35" s="40" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C36" s="42"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="40"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="42"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C37" s="40"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="42" t="s">
+      <c r="C38" s="40" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="42" t="s">
+      <c r="C39" s="40" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="42" t="s">
+      <c r="C40" s="40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="42" t="s">
+      <c r="C41" s="40" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C42" s="42"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="40"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C43" s="42"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C43" s="40"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="42" t="s">
+      <c r="C44" s="40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="42" t="s">
+      <c r="C45" s="40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="42" t="s">
+      <c r="C46" s="40" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="43"/>
-      <c r="B47" s="43" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="41"/>
+      <c r="B47" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="C47" s="44" t="s">
+      <c r="C47" s="42" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2755,505 +2751,472 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7559BD21-F230-4BA5-919B-45F3A616B79F}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="108" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.36328125" customWidth="1"/>
-    <col min="4" max="4" width="19.36328125" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" customWidth="1"/>
-    <col min="6" max="6" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="58"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="62" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="65"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="63" t="s">
+      <c r="E2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="55" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="51" t="s">
         <v>59</v>
       </c>
       <c r="F3" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="50" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="42">
+      <c r="F4" s="40">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="50" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="49" t="s">
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="42">
+      <c r="F5" s="40">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="53" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43" t="s">
+      <c r="B6" s="41"/>
+      <c r="C6" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="43" t="s">
+      <c r="D6" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="44">
+      <c r="F6" s="42">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="56" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="58"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="59" t="s">
+      <c r="B9" s="64"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="65"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="60" t="s">
+      <c r="D10" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="61" t="s">
+      <c r="F10" s="55" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="55" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54" t="s">
+      <c r="B11" s="51"/>
+      <c r="C11" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="54" t="s">
+      <c r="E11" s="51" t="s">
         <v>58</v>
       </c>
       <c r="F11" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="50"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="47"/>
+      <c r="C12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="42">
+      <c r="F12" s="40">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="53"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="50"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="44">
+      <c r="F13" s="42">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="50"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="42"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="55" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="47"/>
+      <c r="F14" s="40"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54" t="s">
+      <c r="B15" s="51"/>
+      <c r="C15" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="54" t="s">
+      <c r="D15" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="54" t="s">
+      <c r="E15" s="51" t="s">
         <v>58</v>
       </c>
       <c r="F15" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="50"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="47"/>
+      <c r="C16" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D16" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="49" t="s">
+      <c r="E16" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="42">
+      <c r="F16" s="40">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="53"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="50"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="44">
+      <c r="F17" s="42">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="50"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="42"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="55" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="47"/>
+      <c r="F18" s="40"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54" t="s">
+      <c r="B19" s="51"/>
+      <c r="C19" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="54" t="s">
+      <c r="D19" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="54" t="s">
+      <c r="E19" s="51" t="s">
         <v>58</v>
       </c>
       <c r="F19" s="12">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="50"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="47"/>
+      <c r="C20" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="49" t="s">
+      <c r="E20" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="42">
+      <c r="F20" s="40">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="53"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="50"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="43" t="s">
+      <c r="D21" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="44">
+      <c r="F21" s="42">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="50"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="42"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="55" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="47"/>
+      <c r="F22" s="40"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54" t="s">
+      <c r="B23" s="51"/>
+      <c r="C23" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="54" t="s">
+      <c r="D23" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="54" t="s">
+      <c r="E23" s="51" t="s">
         <v>58</v>
       </c>
       <c r="F23" s="12">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="50"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="49" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="47"/>
+      <c r="C24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="49" t="s">
+      <c r="E24" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="42">
+      <c r="F24" s="40">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="53"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="50"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="43" t="s">
+      <c r="D25" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="43" t="s">
+      <c r="E25" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="44">
+      <c r="F25" s="42">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="68" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="70"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="62" t="s">
+      <c r="B28" s="67"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="63" t="s">
+      <c r="B29" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="64" t="s">
+      <c r="C29" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="71"/>
-      <c r="E29" s="72"/>
-      <c r="F29" s="73"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="54"/>
+      <c r="B30" s="51"/>
       <c r="C30" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="50" t="s">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="49"/>
-      <c r="C31" s="42" t="s">
+      <c r="C31" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="50" t="s">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="49"/>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="53" t="s">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="44" t="s">
+      <c r="B33" s="41"/>
+      <c r="C33" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="56" t="s">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="57"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="58"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="62" t="s">
+      <c r="B36" s="64"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="65"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="63" t="s">
+      <c r="B37" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="63" t="s">
+      <c r="C37" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="63" t="s">
+      <c r="D37" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="63" t="s">
+      <c r="E37" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="64" t="s">
+      <c r="F37" s="55" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="54"/>
-      <c r="C38" s="54" t="s">
+      <c r="B38" s="51"/>
+      <c r="C38" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="54" t="s">
+      <c r="D38" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="54"/>
+      <c r="E38" s="51"/>
       <c r="F38" s="12">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="53" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="43"/>
-      <c r="C39" s="43" t="s">
+      <c r="B39" s="41"/>
+      <c r="C39" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="43" t="s">
+      <c r="D39" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="43"/>
-      <c r="F39" s="44">
+      <c r="E39" s="41"/>
+      <c r="F39" s="42">
         <v>60</v>
       </c>
     </row>

</xml_diff>